<commit_message>
html and mail and license
</commit_message>
<xml_diff>
--- a/DataSheet/FOS.xlsx
+++ b/DataSheet/FOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B032FA49-181E-4E23-977F-188078A46D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43258A3-93E0-4EA1-9D1F-642287949936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +346,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -370,6 +376,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,7 +1259,7 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">

</xml_diff>

<commit_message>
add maven dependency for making java simply command maven clean maven clean install maven package
</commit_message>
<xml_diff>
--- a/DataSheet/FOS.xlsx
+++ b/DataSheet/FOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43258A3-93E0-4EA1-9D1F-642287949936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CF482-F508-466C-A5C0-4710B5C5C068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
   <si>
     <t>Si_No</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>CheckVisibility</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -694,7 +700,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,7 +1134,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -1172,7 +1178,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1251,7 +1257,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1295,7 +1301,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1339,7 +1345,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1374,7 +1380,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -1418,7 +1424,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1491,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes on html file and write all script for consent
</commit_message>
<xml_diff>
--- a/DataSheet/FOS.xlsx
+++ b/DataSheet/FOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CF482-F508-466C-A5C0-4710B5C5C068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55E80B7-D395-4BBE-AF24-7FB2277E32B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="173">
   <si>
     <t>Si_No</t>
   </si>
@@ -88,18 +88,9 @@
     <t>TC_01_01</t>
   </si>
   <si>
-    <t xml:space="preserve"> FOS login Functionality</t>
-  </si>
-  <si>
-    <t>Open FOS login page</t>
-  </si>
-  <si>
     <t>TC_01_01_01</t>
   </si>
   <si>
-    <t>User redirect to login page</t>
-  </si>
-  <si>
     <t>user enter first pin</t>
   </si>
   <si>
@@ -139,12 +130,6 @@
     <t>WAIT(2000)</t>
   </si>
   <si>
-    <t>OpenApp_UsingOnlyAppPackage</t>
-  </si>
-  <si>
-    <t>WAIT(4000)</t>
-  </si>
-  <si>
     <t>KeyBoardSendKeys</t>
   </si>
   <si>
@@ -172,9 +157,6 @@
     <t>CLICK</t>
   </si>
   <si>
-    <t>(//*[@class=\"android.view.View\"])[18]</t>
-  </si>
-  <si>
     <t>QUIT</t>
   </si>
   <si>
@@ -223,9 +205,6 @@
     <t>Wait 2 second</t>
   </si>
   <si>
-    <t>Wait 4 second</t>
-  </si>
-  <si>
     <t>DriverStart</t>
   </si>
   <si>
@@ -238,83 +217,341 @@
     <t>TC_01_01_08</t>
   </si>
   <si>
+    <t>Wait 5 second</t>
+  </si>
+  <si>
+    <t>Click on Application ID Tab</t>
+  </si>
+  <si>
+    <t>Quit Application</t>
+  </si>
+  <si>
+    <t>Click on Lead</t>
+  </si>
+  <si>
+    <t>TC_01_02</t>
+  </si>
+  <si>
+    <t>TC_01_02_01</t>
+  </si>
+  <si>
+    <t>TC_01_02_02</t>
+  </si>
+  <si>
+    <t>TC_01_02_03</t>
+  </si>
+  <si>
+    <t>ExecutionStart Count Time</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>START_APPLICATION</t>
+  </si>
+  <si>
+    <t>Verify Application button are display</t>
+  </si>
+  <si>
+    <t>Verify Specific Lead are display</t>
+  </si>
+  <si>
+    <t>CheckVisibility</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>//*[@bounds='[55,553][1025,1158]']</t>
+  </si>
+  <si>
+    <t>//android.view.View[contains(@content-desc,'Consent')]</t>
+  </si>
+  <si>
+    <t>(//android.view.View[contains(@content-desc,'Applicant')])[2]</t>
+  </si>
+  <si>
+    <t>(//android.view.View[@content-desc="Primary Details"])[1]</t>
+  </si>
+  <si>
+    <t>(//android.view.View[@content-desc="Mode Of Consent"])[1]</t>
+  </si>
+  <si>
+    <t>//android.view.View[@content-desc="Form"]/android.widget.RadioButton</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@content-desc="Capture Image"]</t>
+  </si>
+  <si>
+    <t>//android.view.View[@content-desc='Add Image']</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>ScrollDown</t>
+  </si>
+  <si>
+    <t>Applicant Consent</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FOS Application Functionality</t>
+  </si>
+  <si>
+    <t>TC_01_03</t>
+  </si>
+  <si>
+    <t>TC_01_04</t>
+  </si>
+  <si>
+    <t>TC_01_03_01</t>
+  </si>
+  <si>
+    <t>TC_01_03_02</t>
+  </si>
+  <si>
+    <t>TC_01_03_03</t>
+  </si>
+  <si>
+    <t>TC_01_03_04</t>
+  </si>
+  <si>
+    <t>TC_01_03_05</t>
+  </si>
+  <si>
+    <t>Verify 'APPLICANT' tab are clicked</t>
+  </si>
+  <si>
+    <t>Click on 'Applicant' tab</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>Application Page</t>
+  </si>
+  <si>
+    <t>Applicant Consent Page</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>TC_01_04_01</t>
+  </si>
+  <si>
+    <t>TC_01_04_02</t>
+  </si>
+  <si>
+    <t>TC_01_04_03</t>
+  </si>
+  <si>
+    <t>TC_01_04_04</t>
+  </si>
+  <si>
+    <t>TC_01_04_05</t>
+  </si>
+  <si>
+    <t>TC_01_04_06</t>
+  </si>
+  <si>
+    <t>TC_01_04_07</t>
+  </si>
+  <si>
+    <t>TC_01_04_08</t>
+  </si>
+  <si>
+    <t>TC_01_04_09</t>
+  </si>
+  <si>
+    <t>TC_01_04_10</t>
+  </si>
+  <si>
+    <t>TC_01_04_11</t>
+  </si>
+  <si>
+    <t>TC_01_04_12</t>
+  </si>
+  <si>
+    <t>TC_01_04_13</t>
+  </si>
+  <si>
+    <t>TC_01_04_14</t>
+  </si>
+  <si>
+    <t>TC_01_04_15</t>
+  </si>
+  <si>
+    <t>TC_01_04_16</t>
+  </si>
+  <si>
+    <t>TC_01_04_17</t>
+  </si>
+  <si>
+    <t>TC_01_04_18</t>
+  </si>
+  <si>
+    <t>TC_01_04_19</t>
+  </si>
+  <si>
+    <t>TC_01_04_20</t>
+  </si>
+  <si>
+    <t>Verify "CONSENT" tab are clickable</t>
+  </si>
+  <si>
+    <t>Click on "CONSENT" Tab</t>
+  </si>
+  <si>
+    <t>Verify "Primary Details" are Displayed</t>
+  </si>
+  <si>
+    <t>Close "Primary Details" Section</t>
+  </si>
+  <si>
+    <t>Open "Mode Of Consent" Section</t>
+  </si>
+  <si>
+    <t>Verify "mode of consent" type</t>
+  </si>
+  <si>
+    <t>Select "Mode Of Consent" is 'Form' based</t>
+  </si>
+  <si>
+    <t>ScrollDown Page</t>
+  </si>
+  <si>
+    <t>Clcik on "Capture Image" Button</t>
+  </si>
+  <si>
+    <t>Click on "Add Image" Button</t>
+  </si>
+  <si>
+    <t>Click on "Save Document" Button</t>
+  </si>
+  <si>
+    <t>Click on "Save and Upload" Button</t>
+  </si>
+  <si>
+    <t>Verify "Save Document" button is display and clickable</t>
+  </si>
+  <si>
+    <t>Verify "Save and Upload" button is display and clickable</t>
+  </si>
+  <si>
+    <t>Verify "Capture Image" button is display and clickable</t>
+  </si>
+  <si>
+    <t>Click on "Proceed" Button</t>
+  </si>
+  <si>
+    <t>Verify after fill all details of consent "Proceed" button are enable</t>
+  </si>
+  <si>
+    <t>Verify "Consent Successfylly Pop_Up Proceed" button are display</t>
+  </si>
+  <si>
+    <t>Click on "Consent Successfully Pop-up Proceed" Button</t>
+  </si>
+  <si>
+    <t>WAIT(6000)</t>
+  </si>
+  <si>
+    <t>Wait 6 second</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@content-desc='Save Document']</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@content-desc='Save and Upload']</t>
+  </si>
+  <si>
+    <t>//android.widget.Button[@content-desc='Proceed']</t>
+  </si>
+  <si>
+    <t>//android.widget.ImageView[@index='0']</t>
+  </si>
+  <si>
     <t>TC_01_01_09</t>
   </si>
   <si>
-    <t>TC_01_01_10</t>
-  </si>
-  <si>
-    <t>Wait 5 second</t>
-  </si>
-  <si>
-    <t>Click on Application ID Tab</t>
-  </si>
-  <si>
-    <t>Quit Application</t>
-  </si>
-  <si>
-    <t>Click on Lead</t>
-  </si>
-  <si>
-    <t>TC_01_02</t>
-  </si>
-  <si>
-    <t>FOS Home Page</t>
-  </si>
-  <si>
-    <t>TC_01_02_01</t>
-  </si>
-  <si>
-    <t>TC_01_02_02</t>
-  </si>
-  <si>
-    <t>TC_01_02_03</t>
-  </si>
-  <si>
-    <t>TC_01_02_04</t>
-  </si>
-  <si>
-    <t>TC_01_02_05</t>
-  </si>
-  <si>
-    <t>ExecutionStart Count Time</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>START_APPLICATION</t>
-  </si>
-  <si>
-    <t>Verify Application button are display</t>
-  </si>
-  <si>
-    <t>Verify Specific Lead are display</t>
-  </si>
-  <si>
-    <t>TC_01_02_06</t>
-  </si>
-  <si>
-    <t>TC_01_02_07</t>
-  </si>
-  <si>
-    <t>CheckVisibility</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>Verify "Mahidra Finance" logo are Displayed</t>
+  </si>
+  <si>
+    <t>37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +578,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,18 +594,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -370,11 +625,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF0F0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -383,6 +647,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,29 +966,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="56.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -771,7 +1040,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -783,30 +1052,30 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L2" t="s">
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -818,30 +1087,30 @@
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L3" t="s">
         <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -849,34 +1118,34 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L4" t="s">
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -884,34 +1153,43 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>85</v>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L5" t="s">
         <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -922,31 +1200,34 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
-        <v>38</v>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L6" t="s">
         <v>19</v>
       </c>
       <c r="M6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
         <v>21</v>
-      </c>
-      <c r="N6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -958,33 +1239,33 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
         <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -996,33 +1277,33 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
         <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
       </c>
       <c r="M8" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -1034,33 +1315,33 @@
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
         <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L9" t="s">
         <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -1071,347 +1352,1227 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" t="s">
-        <v>43</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
         <v>17</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L10" t="s">
         <v>19</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>124</v>
       </c>
       <c r="N10" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="M11" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="N11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M12" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="N12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="O12" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M13" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="N13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
+        <v>89</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
       </c>
       <c r="K14" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" t="s">
+        <v>114</v>
+      </c>
+      <c r="O14" t="s">
         <v>76</v>
-      </c>
-      <c r="M14" t="s">
-        <v>77</v>
-      </c>
-      <c r="N14" t="s">
-        <v>80</v>
-      </c>
-      <c r="O14" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="J15" t="s">
         <v>17</v>
       </c>
       <c r="K15" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L15" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="M15" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="N15" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="O15" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>32</v>
+        <v>89</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="J16" t="s">
         <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L16" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="M16" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="N16" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
       <c r="H17" s="1" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="J17" t="s">
         <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="M17" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="N17" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="O17" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" t="s">
+        <v>118</v>
+      </c>
+      <c r="O18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>111</v>
+      </c>
+      <c r="L19" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19" t="s">
+        <v>123</v>
+      </c>
+      <c r="N19" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" t="s">
-        <v>76</v>
-      </c>
-      <c r="M18" t="s">
-        <v>74</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" t="s">
+        <v>111</v>
+      </c>
+      <c r="L20" t="s">
+        <v>113</v>
+      </c>
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+      <c r="N20" t="s">
+        <v>126</v>
+      </c>
+      <c r="O20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21" t="s">
+        <v>123</v>
+      </c>
+      <c r="N21" t="s">
+        <v>127</v>
+      </c>
+      <c r="O21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22" t="s">
+        <v>123</v>
+      </c>
+      <c r="N22" t="s">
+        <v>128</v>
+      </c>
+      <c r="O22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" t="s">
+        <v>111</v>
+      </c>
+      <c r="L23" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" t="s">
+        <v>123</v>
+      </c>
+      <c r="N23" t="s">
+        <v>129</v>
+      </c>
+      <c r="O23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L24" t="s">
+        <v>113</v>
+      </c>
+      <c r="M24" t="s">
+        <v>123</v>
+      </c>
+      <c r="N24" t="s">
+        <v>130</v>
+      </c>
+      <c r="O24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" t="s">
+        <v>111</v>
+      </c>
+      <c r="L25" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" t="s">
+        <v>123</v>
+      </c>
+      <c r="N25" t="s">
+        <v>131</v>
+      </c>
+      <c r="O25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" t="s">
         <v>90</v>
       </c>
-      <c r="O18" t="s">
-        <v>74</v>
-      </c>
+      <c r="J26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" t="s">
+        <v>111</v>
+      </c>
+      <c r="L26" t="s">
+        <v>113</v>
+      </c>
+      <c r="M26" t="s">
+        <v>123</v>
+      </c>
+      <c r="N26" t="s">
+        <v>132</v>
+      </c>
+      <c r="O26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" t="s">
+        <v>111</v>
+      </c>
+      <c r="L27" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" t="s">
+        <v>123</v>
+      </c>
+      <c r="N27" t="s">
+        <v>133</v>
+      </c>
+      <c r="O27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" t="s">
+        <v>111</v>
+      </c>
+      <c r="L28" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" t="s">
+        <v>134</v>
+      </c>
+      <c r="O28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" t="s">
+        <v>111</v>
+      </c>
+      <c r="L29" t="s">
+        <v>113</v>
+      </c>
+      <c r="M29" t="s">
+        <v>123</v>
+      </c>
+      <c r="N29" t="s">
+        <v>135</v>
+      </c>
+      <c r="O29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J30" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" t="s">
+        <v>111</v>
+      </c>
+      <c r="L30" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30" t="s">
+        <v>123</v>
+      </c>
+      <c r="N30" t="s">
+        <v>136</v>
+      </c>
+      <c r="O30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L31" t="s">
+        <v>113</v>
+      </c>
+      <c r="M31" t="s">
+        <v>123</v>
+      </c>
+      <c r="N31" t="s">
+        <v>137</v>
+      </c>
+      <c r="O31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" t="s">
+        <v>111</v>
+      </c>
+      <c r="L32" t="s">
+        <v>113</v>
+      </c>
+      <c r="M32" t="s">
+        <v>123</v>
+      </c>
+      <c r="N32" t="s">
+        <v>138</v>
+      </c>
+      <c r="O32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" t="s">
+        <v>111</v>
+      </c>
+      <c r="L33" t="s">
+        <v>113</v>
+      </c>
+      <c r="M33" t="s">
+        <v>123</v>
+      </c>
+      <c r="N33" t="s">
+        <v>139</v>
+      </c>
+      <c r="O33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J34" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L34" t="s">
+        <v>113</v>
+      </c>
+      <c r="M34" t="s">
+        <v>123</v>
+      </c>
+      <c r="N34" t="s">
+        <v>140</v>
+      </c>
+      <c r="O34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" t="s">
+        <v>111</v>
+      </c>
+      <c r="L35" t="s">
+        <v>113</v>
+      </c>
+      <c r="M35" t="s">
+        <v>123</v>
+      </c>
+      <c r="N35" t="s">
+        <v>141</v>
+      </c>
+      <c r="O35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" t="s">
+        <v>111</v>
+      </c>
+      <c r="L36" t="s">
+        <v>113</v>
+      </c>
+      <c r="M36" t="s">
+        <v>123</v>
+      </c>
+      <c r="N36" t="s">
+        <v>142</v>
+      </c>
+      <c r="O36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" t="s">
+        <v>111</v>
+      </c>
+      <c r="L37" t="s">
+        <v>113</v>
+      </c>
+      <c r="M37" t="s">
+        <v>123</v>
+      </c>
+      <c r="N37" t="s">
+        <v>143</v>
+      </c>
+      <c r="O37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" t="s">
+        <v>111</v>
+      </c>
+      <c r="L38" t="s">
+        <v>113</v>
+      </c>
+      <c r="M38" t="s">
+        <v>65</v>
+      </c>
+      <c r="N38" t="s">
+        <v>144</v>
+      </c>
+      <c r="O38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F42" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1444,25 +2605,25 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1491,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="I2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change some datasheet and maincontroller file
</commit_message>
<xml_diff>
--- a/DataSheet/FOS.xlsx
+++ b/DataSheet/FOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BSA_MOBILE_FRAMEWORK\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697A5387-0B95-4545-B173-DE3BB028E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185C5BAD-A295-4AEC-9125-17F9CE21ADBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875AE543-1650-41B3-9C38-4B818EB686AA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="199">
   <si>
     <t>Si_No</t>
   </si>
@@ -548,9 +548,6 @@
   </si>
   <si>
     <t>//android.widget.Button[@content-desc='Set MPIN']</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>/hierarchy/android.widget.FrameLayout/android.widget.LinearLayout/android.widget.FrameLayout/android.widget.FrameLayout/android.view.View/android.view.View/android.view.View/android.widget.ScrollView/android.widget.EditText[2]</t>
@@ -617,10 +614,16 @@
     <t>cameraImageInjection</t>
   </si>
   <si>
-    <t>media://fbb291007ac2f3d6c5d56787d75740f5175aba2a</t>
-  </si>
-  <si>
     <t>WAIT(40000)</t>
+  </si>
+  <si>
+    <t>eb16da7fbca4fa417259747aa7baab4fa04aa4c5</t>
+  </si>
+  <si>
+    <t>ApplicantPanUploadImage</t>
+  </si>
+  <si>
+    <t>ae9508caeddeebeba6bdee241061a4e654109793</t>
   </si>
 </sst>
 </file>
@@ -669,7 +672,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,12 +694,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5F5F5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,7 +720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -735,7 +732,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1055,10 +1051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0CA32F-6895-4985-AF4D-119BC41D4938}">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="74" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="74" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1827,7 +1823,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J18" t="s">
         <v>17</v>
@@ -2215,7 +2211,7 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>170</v>
@@ -2339,7 +2335,7 @@
       </c>
       <c r="F30" s="6"/>
       <c r="H30" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J30" t="s">
         <v>17</v>
@@ -2377,7 +2373,7 @@
         <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>171</v>
@@ -2506,7 +2502,7 @@
         <v>37</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G34" t="s">
         <v>30</v>
@@ -2543,14 +2539,14 @@
       <c r="C35" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G35" t="s">
         <v>29</v>
@@ -2592,7 +2588,7 @@
       </c>
       <c r="F36" s="6"/>
       <c r="H36" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J36" t="s">
         <v>17</v>
@@ -2623,14 +2619,14 @@
       <c r="C37" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" t="s">
         <v>16</v>
       </c>
       <c r="E37" t="s">
         <v>37</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G37" t="s">
         <v>30</v>
@@ -2667,14 +2663,14 @@
       <c r="C38" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="9" t="s">
-        <v>180</v>
+      <c r="F38" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="G38" t="s">
         <v>29</v>
@@ -2718,7 +2714,7 @@
         <v>37</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G39" t="s">
         <v>30</v>
@@ -2762,7 +2758,7 @@
         <v>37</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G40" t="s">
         <v>29</v>
@@ -2806,7 +2802,7 @@
         <v>37</v>
       </c>
       <c r="F41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G41" t="s">
         <v>30</v>
@@ -2850,7 +2846,7 @@
         <v>37</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G42" t="s">
         <v>29</v>
@@ -2894,7 +2890,7 @@
         <v>37</v>
       </c>
       <c r="F43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G43" t="s">
         <v>30</v>
@@ -2938,7 +2934,7 @@
         <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G44" t="s">
         <v>29</v>
@@ -2982,7 +2978,7 @@
         <v>37</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G45" t="s">
         <v>30</v>
@@ -3026,7 +3022,7 @@
         <v>37</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G46" t="s">
         <v>29</v>
@@ -3070,7 +3066,7 @@
         <v>37</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G47" t="s">
         <v>29</v>
@@ -3114,7 +3110,7 @@
         <v>37</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G48" t="s">
         <v>30</v>
@@ -3158,7 +3154,7 @@
         <v>37</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G49" t="s">
         <v>29</v>
@@ -3235,10 +3231,10 @@
       </c>
       <c r="F51" s="6"/>
       <c r="G51" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51" t="s">
         <v>194</v>
-      </c>
-      <c r="H51" t="s">
-        <v>195</v>
       </c>
       <c r="J51" t="s">
         <v>17</v>
@@ -3276,7 +3272,7 @@
         <v>37</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G52" t="s">
         <v>30</v>
@@ -3320,7 +3316,7 @@
         <v>37</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G53" t="s">
         <v>29</v>
@@ -3347,9 +3343,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B54" t="s">
         <v>15</v>
@@ -3360,12 +3356,17 @@
       <c r="D54" t="s">
         <v>16</v>
       </c>
-      <c r="F54" s="6"/>
+      <c r="E54" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" t="s">
+        <v>187</v>
+      </c>
       <c r="G54" t="s">
-        <v>194</v>
-      </c>
-      <c r="H54" t="s">
-        <v>195</v>
+        <v>29</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="J54" t="s">
         <v>17</v>
@@ -3380,15 +3381,15 @@
         <v>110</v>
       </c>
       <c r="N54" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O54" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
@@ -3402,14 +3403,14 @@
       <c r="E55" t="s">
         <v>37</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>188</v>
       </c>
       <c r="G55" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="J55" t="s">
         <v>17</v>
@@ -3424,15 +3425,15 @@
         <v>110</v>
       </c>
       <c r="N55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O55" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
@@ -3447,13 +3448,13 @@
         <v>37</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G56" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="J56" t="s">
         <v>17</v>
@@ -3468,15 +3469,15 @@
         <v>110</v>
       </c>
       <c r="N56" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
@@ -3494,10 +3495,10 @@
         <v>189</v>
       </c>
       <c r="G57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="J57" t="s">
         <v>17</v>
@@ -3512,15 +3513,15 @@
         <v>110</v>
       </c>
       <c r="N57" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O57" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
@@ -3535,13 +3536,13 @@
         <v>37</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="J58" t="s">
         <v>17</v>
@@ -3556,15 +3557,15 @@
         <v>110</v>
       </c>
       <c r="N58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -3582,10 +3583,10 @@
         <v>190</v>
       </c>
       <c r="G59" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="J59" t="s">
         <v>17</v>
@@ -3600,15 +3601,15 @@
         <v>110</v>
       </c>
       <c r="N59" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O59" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
@@ -3623,13 +3624,13 @@
         <v>37</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="J60" t="s">
         <v>17</v>
@@ -3644,15 +3645,15 @@
         <v>110</v>
       </c>
       <c r="N60" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
@@ -3660,20 +3661,20 @@
       <c r="C61" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>174</v>
+      <c r="D61" t="s">
+        <v>16</v>
       </c>
       <c r="E61" t="s">
         <v>37</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G61" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="J61" t="s">
         <v>17</v>
@@ -3688,15 +3689,15 @@
         <v>110</v>
       </c>
       <c r="N61" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O61" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
@@ -3704,151 +3705,454 @@
       <c r="C62" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>174</v>
+      <c r="D62" t="s">
+        <v>16</v>
       </c>
       <c r="E62" t="s">
         <v>37</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G62" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J62" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" t="s">
+        <v>98</v>
+      </c>
+      <c r="L62" t="s">
+        <v>100</v>
+      </c>
+      <c r="M62" t="s">
+        <v>110</v>
+      </c>
+      <c r="N62" t="s">
+        <v>130</v>
+      </c>
+      <c r="O62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" t="s">
+        <v>197</v>
+      </c>
+      <c r="H63" t="s">
+        <v>194</v>
+      </c>
+      <c r="J63" t="s">
+        <v>17</v>
+      </c>
+      <c r="K63" t="s">
+        <v>98</v>
+      </c>
+      <c r="L63" t="s">
+        <v>100</v>
+      </c>
+      <c r="M63" t="s">
+        <v>110</v>
+      </c>
+      <c r="N63" t="s">
+        <v>120</v>
+      </c>
+      <c r="O63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G64" t="s">
         <v>30</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J62" t="s">
-        <v>17</v>
-      </c>
-      <c r="K62" t="s">
-        <v>98</v>
-      </c>
-      <c r="L62" t="s">
-        <v>100</v>
-      </c>
-      <c r="M62" t="s">
-        <v>110</v>
-      </c>
-      <c r="N62" t="s">
-        <v>129</v>
-      </c>
-      <c r="O62" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" t="s">
-        <v>78</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" t="s">
-        <v>37</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G63" t="s">
+      <c r="J64" t="s">
+        <v>17</v>
+      </c>
+      <c r="K64" t="s">
+        <v>98</v>
+      </c>
+      <c r="L64" t="s">
+        <v>100</v>
+      </c>
+      <c r="M64" t="s">
+        <v>110</v>
+      </c>
+      <c r="N64" t="s">
+        <v>120</v>
+      </c>
+      <c r="O64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G65" t="s">
         <v>29</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H65" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J63" t="s">
-        <v>17</v>
-      </c>
-      <c r="K63" t="s">
-        <v>98</v>
-      </c>
-      <c r="L63" t="s">
-        <v>100</v>
-      </c>
-      <c r="M63" t="s">
-        <v>110</v>
-      </c>
-      <c r="N63" t="s">
-        <v>130</v>
-      </c>
-      <c r="O63" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+      <c r="J65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K65" t="s">
+        <v>98</v>
+      </c>
+      <c r="L65" t="s">
+        <v>100</v>
+      </c>
+      <c r="M65" t="s">
+        <v>110</v>
+      </c>
+      <c r="N65" t="s">
+        <v>121</v>
+      </c>
+      <c r="O65" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>37</v>
+      </c>
+      <c r="F66" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J66" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" t="s">
+        <v>98</v>
+      </c>
+      <c r="L66" t="s">
+        <v>100</v>
+      </c>
+      <c r="M66" t="s">
+        <v>110</v>
+      </c>
+      <c r="N66" t="s">
+        <v>122</v>
+      </c>
+      <c r="O66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" t="s">
+        <v>37</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J67" t="s">
+        <v>17</v>
+      </c>
+      <c r="K67" t="s">
+        <v>98</v>
+      </c>
+      <c r="L67" t="s">
+        <v>100</v>
+      </c>
+      <c r="M67" t="s">
+        <v>110</v>
+      </c>
+      <c r="N67" t="s">
+        <v>123</v>
+      </c>
+      <c r="O67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>78</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G68" t="s">
+        <v>29</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J68" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" t="s">
+        <v>98</v>
+      </c>
+      <c r="L68" t="s">
+        <v>100</v>
+      </c>
+      <c r="M68" t="s">
+        <v>110</v>
+      </c>
+      <c r="N68" t="s">
+        <v>124</v>
+      </c>
+      <c r="O68" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>37</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G69" t="s">
+        <v>30</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J69" t="s">
+        <v>17</v>
+      </c>
+      <c r="K69" t="s">
+        <v>98</v>
+      </c>
+      <c r="L69" t="s">
+        <v>100</v>
+      </c>
+      <c r="M69" t="s">
+        <v>110</v>
+      </c>
+      <c r="N69" t="s">
+        <v>125</v>
+      </c>
+      <c r="O69" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>78</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>37</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G70" t="s">
+        <v>29</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J70" t="s">
+        <v>17</v>
+      </c>
+      <c r="K70" t="s">
+        <v>98</v>
+      </c>
+      <c r="L70" t="s">
+        <v>100</v>
+      </c>
+      <c r="M70" t="s">
+        <v>110</v>
+      </c>
+      <c r="N70" t="s">
+        <v>126</v>
+      </c>
+      <c r="O70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
         <v>76</v>
       </c>
-      <c r="D64" t="s">
-        <v>16</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="J64" t="s">
-        <v>17</v>
-      </c>
-      <c r="K64" t="s">
-        <v>98</v>
-      </c>
-      <c r="L64" t="s">
-        <v>100</v>
-      </c>
-      <c r="M64" t="s">
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J71" t="s">
+        <v>17</v>
+      </c>
+      <c r="K71" t="s">
+        <v>98</v>
+      </c>
+      <c r="L71" t="s">
+        <v>100</v>
+      </c>
+      <c r="M71" t="s">
         <v>61</v>
       </c>
-      <c r="N64" t="s">
+      <c r="N71" t="s">
         <v>131</v>
       </c>
-      <c r="O64" t="s">
+      <c r="O71" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
         <v>76</v>
       </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-      <c r="H65" s="1" t="s">
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J65" t="s">
-        <v>17</v>
-      </c>
-      <c r="K65" t="s">
-        <v>98</v>
-      </c>
-      <c r="L65" t="s">
-        <v>100</v>
-      </c>
-      <c r="M65" t="s">
+      <c r="J72" t="s">
+        <v>17</v>
+      </c>
+      <c r="K72" t="s">
+        <v>98</v>
+      </c>
+      <c r="L72" t="s">
+        <v>100</v>
+      </c>
+      <c r="M72" t="s">
         <v>61</v>
       </c>
-      <c r="N65" t="s">
+      <c r="N72" t="s">
         <v>131</v>
       </c>
-      <c r="O65" t="s">
+      <c r="O72" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3860,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A86AEA-BDCA-4ACF-93E7-52FBBDAF5EE7}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3876,7 +4180,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3911,13 +4215,16 @@
         <v>167</v>
       </c>
       <c r="L1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+      <c r="N1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3948,14 +4255,17 @@
       <c r="J2">
         <v>100005561</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>168</v>
       </c>
       <c r="L2">
         <v>4</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
         <v>196</v>
+      </c>
+      <c r="N2" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>